<commit_message>
1.add the abnormal flag in result 2.add the max and min predict data
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7275"/>
   </bookViews>
   <sheets>
-    <sheet name="clause" sheetId="1" r:id="rId1"/>
+    <sheet name="clause" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -71,6 +72,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -81,6 +83,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -93,6 +96,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -103,6 +107,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -115,6 +120,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -125,6 +131,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -137,6 +144,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -147,6 +155,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,6 +168,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -169,6 +179,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -181,6 +192,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -191,6 +203,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -203,6 +216,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -213,6 +227,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -225,6 +240,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -235,6 +251,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -292,23 +309,23 @@
       </rPr>
       <t>eining</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>qiangli</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>ruifeng</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>zhengdan</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>xinru</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -330,35 +347,165 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>123104</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sz123076</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sz123126</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sz123106</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sz128142</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lepu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xianglu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruida</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>daoen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinbo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xianggang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>huati</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123108</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128072</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">128116 </t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2026/06/28</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128117</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">118001 </t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>113566</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh113574</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>scale</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,27 +520,22 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -435,16 +577,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -505,7 +645,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,7 +680,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,19 +889,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J2" sqref="J2:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,10 +929,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -817,11 +958,14 @@
       <c r="H2">
         <v>15</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>46016</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J2">
+        <v>2.2170000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -846,11 +990,14 @@
       <c r="H3">
         <v>18</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>46224</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J3">
+        <v>2.496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -875,11 +1022,14 @@
       <c r="H4">
         <v>24</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>46405</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J4">
+        <v>2.4849999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -904,11 +1054,14 @@
       <c r="H5">
         <v>15</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>46196</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J5">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -933,11 +1086,14 @@
       <c r="H6">
         <v>15</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>45832</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J6">
+        <v>2.9940000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -962,11 +1118,14 @@
       <c r="H7">
         <v>10</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>46560</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J7">
+        <v>9.9990000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -991,11 +1150,14 @@
       <c r="H8">
         <v>15</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>46268</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J8">
+        <v>2.1890000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1020,11 +1182,14 @@
       <c r="H9">
         <v>14</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>45491</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J9">
+        <v>2.5059999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1049,11 +1214,14 @@
       <c r="H10">
         <v>21.5</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>46092</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J10">
+        <v>5.4960000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1078,15 +1246,18 @@
       <c r="H11">
         <v>18</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="3">
         <v>46349</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="J11">
+        <v>7.3380000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C12">
@@ -1107,15 +1278,18 @@
       <c r="H12">
         <v>21</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>46412</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+      <c r="J12">
+        <v>8.1690000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C13">
@@ -1136,15 +1310,18 @@
       <c r="H13">
         <v>12</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>45736</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="J13">
+        <v>5.2939999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C14">
@@ -1165,21 +1342,24 @@
       <c r="H14">
         <v>21</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="3">
         <v>46124</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+      <c r="J14">
+        <v>9.17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C15">
         <v>0.3</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15">
         <v>0.5</v>
       </c>
       <c r="E15">
@@ -1194,21 +1374,24 @@
       <c r="H15">
         <v>20</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="3">
         <v>46461</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
+      <c r="J15">
+        <v>9.7010000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C16">
         <v>0.4</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16">
         <v>0.6</v>
       </c>
       <c r="E16">
@@ -1223,21 +1406,24 @@
       <c r="H16">
         <v>13</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="3">
         <v>46344</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="J16">
+        <v>8.4990000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C17">
         <v>0.5</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17">
         <v>0.8</v>
       </c>
       <c r="E17">
@@ -1252,21 +1438,24 @@
       <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="3">
         <v>46639</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
+      <c r="J17">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C18">
         <v>0.4</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>0.6</v>
       </c>
       <c r="E18">
@@ -1281,21 +1470,24 @@
       <c r="H18">
         <v>20</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="3">
         <v>46469</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="J18">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C19">
         <v>0.3</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19">
         <v>0.5</v>
       </c>
       <c r="E19">
@@ -1310,16 +1502,261 @@
       <c r="H19">
         <v>10</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="3">
         <v>46373</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="J19">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>0.4</v>
+      </c>
+      <c r="D20">
+        <v>0.6</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1.5</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20" s="3">
+        <v>46204</v>
+      </c>
+      <c r="J20">
+        <v>3.5990000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.8</v>
+      </c>
+      <c r="E21">
+        <v>1.2</v>
+      </c>
+      <c r="F21">
+        <v>1.8</v>
+      </c>
+      <c r="G21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21" s="3">
+        <v>46080</v>
+      </c>
+      <c r="J21">
+        <v>1.613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>0.7</v>
+      </c>
+      <c r="E22">
+        <v>1.2</v>
+      </c>
+      <c r="F22">
+        <v>1.8</v>
+      </c>
+      <c r="G22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3">
+        <v>46111</v>
+      </c>
+      <c r="J22">
+        <v>2.089</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23">
+        <v>0.4</v>
+      </c>
+      <c r="D23">
+        <v>0.6</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1.5</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3">
+        <v>45888</v>
+      </c>
+      <c r="J23">
+        <v>3.0179999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24">
+        <v>0.3</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1.5</v>
+      </c>
+      <c r="G24">
+        <v>1.8</v>
+      </c>
+      <c r="H24">
+        <v>7.8</v>
+      </c>
+      <c r="I24" s="3">
+        <v>46110</v>
+      </c>
+      <c r="J24">
+        <v>16.378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B25" s="2"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B26" s="2"/>
+      <c r="I26" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1">
+        <v>0.4</v>
+      </c>
+      <c r="D1">
+        <v>0.5</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1.5</v>
+      </c>
+      <c r="G1">
+        <v>1.9</v>
+      </c>
+      <c r="H1">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.7</v>
+      </c>
+      <c r="E2">
+        <v>1.2</v>
+      </c>
+      <c r="F2">
+        <v>1.8</v>
+      </c>
+      <c r="G2">
+        <v>2.4</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3">
+        <v>46590</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1.add some items in interest.xlsx
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -497,7 +497,159 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>scale</t>
+    <t>sz128125</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qimo2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>huayang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fenglong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128143</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz127021</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tefa2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128122</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xingsen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz127035</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>punai</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz127034</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lvyin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lege</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123072</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beisi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123075</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sannuo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ouzu</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z128074</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h113593</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hugong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z123133</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>peidi</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -577,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -585,6 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -889,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J24"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -929,9 +1082,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -961,9 +1112,6 @@
       <c r="I2" s="3">
         <v>46016</v>
       </c>
-      <c r="J2">
-        <v>2.2170000000000001</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
@@ -993,9 +1141,6 @@
       <c r="I3" s="3">
         <v>46224</v>
       </c>
-      <c r="J3">
-        <v>2.496</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1025,9 +1170,6 @@
       <c r="I4" s="3">
         <v>46405</v>
       </c>
-      <c r="J4">
-        <v>2.4849999999999999</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
@@ -1057,9 +1199,6 @@
       <c r="I5" s="3">
         <v>46196</v>
       </c>
-      <c r="J5">
-        <v>5.84</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
@@ -1089,9 +1228,6 @@
       <c r="I6" s="3">
         <v>45832</v>
       </c>
-      <c r="J6">
-        <v>2.9940000000000002</v>
-      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
@@ -1121,9 +1257,6 @@
       <c r="I7" s="3">
         <v>46560</v>
       </c>
-      <c r="J7">
-        <v>9.9990000000000006</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
@@ -1153,9 +1286,6 @@
       <c r="I8" s="3">
         <v>46268</v>
       </c>
-      <c r="J8">
-        <v>2.1890000000000001</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
@@ -1185,9 +1315,6 @@
       <c r="I9" s="3">
         <v>45491</v>
       </c>
-      <c r="J9">
-        <v>2.5059999999999998</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
@@ -1217,9 +1344,6 @@
       <c r="I10" s="3">
         <v>46092</v>
       </c>
-      <c r="J10">
-        <v>5.4960000000000004</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
@@ -1249,9 +1373,6 @@
       <c r="I11" s="3">
         <v>46349</v>
       </c>
-      <c r="J11">
-        <v>7.3380000000000001</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
@@ -1281,9 +1402,6 @@
       <c r="I12" s="3">
         <v>46412</v>
       </c>
-      <c r="J12">
-        <v>8.1690000000000005</v>
-      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
@@ -1313,9 +1431,6 @@
       <c r="I13" s="3">
         <v>45736</v>
       </c>
-      <c r="J13">
-        <v>5.2939999999999996</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
@@ -1345,9 +1460,6 @@
       <c r="I14" s="3">
         <v>46124</v>
       </c>
-      <c r="J14">
-        <v>9.17</v>
-      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
@@ -1377,9 +1489,6 @@
       <c r="I15" s="3">
         <v>46461</v>
       </c>
-      <c r="J15">
-        <v>9.7010000000000005</v>
-      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
@@ -1409,11 +1518,8 @@
       <c r="I16" s="3">
         <v>46344</v>
       </c>
-      <c r="J16">
-        <v>8.4990000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1441,11 +1547,8 @@
       <c r="I17" s="3">
         <v>46639</v>
       </c>
-      <c r="J17">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1473,11 +1576,8 @@
       <c r="I18" s="3">
         <v>46469</v>
       </c>
-      <c r="J18">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1505,11 +1605,8 @@
       <c r="I19" s="3">
         <v>46373</v>
       </c>
-      <c r="J19">
-        <v>7.18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1537,11 +1634,8 @@
       <c r="I20" s="3">
         <v>46204</v>
       </c>
-      <c r="J20">
-        <v>3.5990000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1569,11 +1663,8 @@
       <c r="I21" s="3">
         <v>46080</v>
       </c>
-      <c r="J21">
-        <v>1.613</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1601,11 +1692,8 @@
       <c r="I22" s="3">
         <v>46111</v>
       </c>
-      <c r="J22">
-        <v>2.089</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1633,11 +1721,8 @@
       <c r="I23" s="3">
         <v>45888</v>
       </c>
-      <c r="J23">
-        <v>3.0179999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1645,19 +1730,19 @@
         <v>52</v>
       </c>
       <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>0.3</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>0.5</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
       <c r="F24">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="H24">
         <v>7.8</v>
@@ -1665,17 +1750,383 @@
       <c r="I24" s="3">
         <v>46110</v>
       </c>
-      <c r="J24">
-        <v>16.378</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B25" s="2"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B26" s="2"/>
-      <c r="I26" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>0.4</v>
+      </c>
+      <c r="D25">
+        <v>0.6</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1.5</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>13</v>
+      </c>
+      <c r="I25" s="5">
+        <v>46232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>0.3</v>
+      </c>
+      <c r="D26">
+        <v>0.6</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1.5</v>
+      </c>
+      <c r="G26">
+        <v>1.8</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26" s="3">
+        <v>46017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>0.7</v>
+      </c>
+      <c r="E27">
+        <v>1.2</v>
+      </c>
+      <c r="F27">
+        <v>1.8</v>
+      </c>
+      <c r="G27">
+        <v>2.5</v>
+      </c>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27" s="3">
+        <v>46394</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.3</v>
+      </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1.5</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28" s="3">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.3</v>
+      </c>
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1.5</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29" s="3">
+        <v>45860</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.6</v>
+      </c>
+      <c r="E30">
+        <v>0.8</v>
+      </c>
+      <c r="F30">
+        <v>1.5</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I30" s="3">
+        <v>46167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31">
+        <v>0.4</v>
+      </c>
+      <c r="D31">
+        <v>0.6</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1.5</v>
+      </c>
+      <c r="G31">
+        <v>2.5</v>
+      </c>
+      <c r="H31">
+        <v>13</v>
+      </c>
+      <c r="I31" s="3">
+        <v>46506</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <v>0.8</v>
+      </c>
+      <c r="E32">
+        <v>1.8</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>3.5</v>
+      </c>
+      <c r="H32">
+        <v>20</v>
+      </c>
+      <c r="I32" s="3">
+        <v>46315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33">
+        <v>0.4</v>
+      </c>
+      <c r="D33">
+        <v>0.6</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1.5</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33" s="3">
+        <v>46327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34">
+        <v>0.3</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1.5</v>
+      </c>
+      <c r="G34">
+        <v>1.8</v>
+      </c>
+      <c r="H34">
+        <v>12</v>
+      </c>
+      <c r="I34" s="3">
+        <v>46376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35">
+        <v>0.4</v>
+      </c>
+      <c r="D35">
+        <v>0.6</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1.5</v>
+      </c>
+      <c r="G35">
+        <v>1.8</v>
+      </c>
+      <c r="H35">
+        <v>15</v>
+      </c>
+      <c r="I35" s="3">
+        <v>45922</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36">
+        <v>0.4</v>
+      </c>
+      <c r="D36">
+        <v>0.6</v>
+      </c>
+      <c r="E36">
+        <v>1.2</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>2.4</v>
+      </c>
+      <c r="H36">
+        <v>15</v>
+      </c>
+      <c r="I36" s="3">
+        <v>46222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37">
+        <v>0.4</v>
+      </c>
+      <c r="D37">
+        <v>0.6</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1.5</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>15</v>
+      </c>
+      <c r="I37" s="3">
+        <v>46742</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
1.add bank tab page for flowing money 2.add somme items in interest.xlsx
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -650,6 +650,141 @@
   </si>
   <si>
     <t>peidi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lingkang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhongda</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>weige</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>leidi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>liande</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jufei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>puli</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiongdi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tai21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuhan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chenfeng</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh113610</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>127048</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>113527</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123045</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123038</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123050</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiudian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z123110</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123099</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128021</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh113638</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123122</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh113628</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -729,7 +864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -738,6 +873,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1042,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2126,6 +2262,354 @@
       </c>
       <c r="I37" s="3">
         <v>46742</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38">
+        <v>0.4</v>
+      </c>
+      <c r="D38">
+        <v>0.7</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1.5</v>
+      </c>
+      <c r="G38">
+        <v>2.5</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="I38" s="3">
+        <v>46356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39">
+        <v>0.4</v>
+      </c>
+      <c r="D39">
+        <v>0.8</v>
+      </c>
+      <c r="E39">
+        <v>1.2</v>
+      </c>
+      <c r="F39">
+        <v>1.8</v>
+      </c>
+      <c r="G39">
+        <v>2.5</v>
+      </c>
+      <c r="H39">
+        <v>15</v>
+      </c>
+      <c r="I39" s="3">
+        <v>46685</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40">
+        <v>0.7</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1.5</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>15</v>
+      </c>
+      <c r="I40" s="3">
+        <v>45680</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41">
+        <v>0.5</v>
+      </c>
+      <c r="D41">
+        <v>0.7</v>
+      </c>
+      <c r="E41">
+        <v>1.2</v>
+      </c>
+      <c r="F41">
+        <v>1.8</v>
+      </c>
+      <c r="G41">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H41">
+        <v>13</v>
+      </c>
+      <c r="I41" s="3">
+        <v>46092</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42">
+        <v>0.5</v>
+      </c>
+      <c r="D42">
+        <v>0.7</v>
+      </c>
+      <c r="E42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F42">
+        <v>1.7</v>
+      </c>
+      <c r="G42">
+        <v>2.1</v>
+      </c>
+      <c r="H42">
+        <v>13</v>
+      </c>
+      <c r="I42" s="3">
+        <v>46015</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43">
+        <v>0.4</v>
+      </c>
+      <c r="D43">
+        <v>0.8</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1.5</v>
+      </c>
+      <c r="G43">
+        <v>2.5</v>
+      </c>
+      <c r="H43">
+        <v>18</v>
+      </c>
+      <c r="I43" s="3">
+        <v>46125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44">
+        <v>0.4</v>
+      </c>
+      <c r="D44">
+        <v>0.6</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1.5</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>18</v>
+      </c>
+      <c r="I44" s="3">
+        <v>46426</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45">
+        <v>0.3</v>
+      </c>
+      <c r="D45">
+        <v>0.5</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1.3</v>
+      </c>
+      <c r="G45">
+        <v>1.5</v>
+      </c>
+      <c r="H45">
+        <v>6</v>
+      </c>
+      <c r="I45" s="3">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46">
+        <v>0.3</v>
+      </c>
+      <c r="D46">
+        <v>0.5</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1.5</v>
+      </c>
+      <c r="G46">
+        <v>1.8</v>
+      </c>
+      <c r="H46">
+        <v>12</v>
+      </c>
+      <c r="I46" s="3">
+        <v>46749</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47">
+        <v>0.3</v>
+      </c>
+      <c r="D47">
+        <v>0.5</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1.5</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>15</v>
+      </c>
+      <c r="I47" s="3">
+        <v>46604</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+      <c r="D48">
+        <v>0.7</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>2.5</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48" s="3">
+        <v>46621</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49">
+        <v>0.4</v>
+      </c>
+      <c r="D49">
+        <v>0.6</v>
+      </c>
+      <c r="E49">
+        <v>1.2</v>
+      </c>
+      <c r="F49">
+        <v>1.8</v>
+      </c>
+      <c r="G49">
+        <v>2.4</v>
+      </c>
+      <c r="H49">
+        <v>15</v>
+      </c>
+      <c r="I49" s="3">
+        <v>46477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add huazheng，beilu and ruida to interest.xlsx
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>name</t>
   </si>
@@ -785,6 +785,30 @@
   </si>
   <si>
     <t>sh113628</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beilu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123082</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruida</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128116</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>huazheng</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh113639</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1178,15 +1202,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2610,6 +2635,93 @@
       </c>
       <c r="I49" s="3">
         <v>46477</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50">
+        <v>0.5</v>
+      </c>
+      <c r="D50">
+        <v>0.7</v>
+      </c>
+      <c r="E50">
+        <v>1.2</v>
+      </c>
+      <c r="F50">
+        <v>1.8</v>
+      </c>
+      <c r="G50">
+        <v>2.5</v>
+      </c>
+      <c r="H50">
+        <v>15</v>
+      </c>
+      <c r="I50" s="3">
+        <v>46362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51">
+        <v>0.4</v>
+      </c>
+      <c r="D51">
+        <v>0.5</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>1.5</v>
+      </c>
+      <c r="G51">
+        <v>1.9</v>
+      </c>
+      <c r="H51">
+        <v>10</v>
+      </c>
+      <c r="I51" s="3">
+        <v>46201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52">
+        <v>0.2</v>
+      </c>
+      <c r="D52">
+        <v>0.4</v>
+      </c>
+      <c r="E52">
+        <v>0.6</v>
+      </c>
+      <c r="F52">
+        <v>1.5</v>
+      </c>
+      <c r="G52">
+        <v>1.8</v>
+      </c>
+      <c r="H52">
+        <v>8</v>
+      </c>
+      <c r="I52" s="3">
+        <v>46775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add chunzhong and zongheng to interest.xlsx
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Robinson\Harpoon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7275"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
   <si>
     <t>name</t>
   </si>
@@ -72,7 +67,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -83,7 +77,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -96,7 +89,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -107,7 +99,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -120,7 +111,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -131,7 +121,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -144,7 +133,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -155,7 +143,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -168,7 +155,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -179,7 +165,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -192,7 +177,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -203,7 +187,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -216,7 +199,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -227,7 +209,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -240,7 +221,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +231,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -296,6 +275,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>w</t>
     </r>
     <r>
@@ -303,32 +289,246 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>eining</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>123104</t>
+    </r>
   </si>
   <si>
     <t>qiangli</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123076</t>
   </si>
   <si>
     <t>ruifeng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123126</t>
   </si>
   <si>
     <t>zhengdan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz123106</t>
   </si>
   <si>
     <t>xinru</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
+  </si>
+  <si>
+    <t>sz128142</t>
+  </si>
+  <si>
+    <t>daoen</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128117</t>
+    </r>
+  </si>
+  <si>
+    <t>xianggang</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>113566</t>
+    </r>
+  </si>
+  <si>
+    <t>huati</t>
+  </si>
+  <si>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>xianglu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128072</t>
+    </r>
+  </si>
+  <si>
+    <t>lepu2</t>
+  </si>
+  <si>
+    <t>sz123108</t>
+  </si>
+  <si>
+    <t>huayang</t>
+  </si>
+  <si>
+    <t>sz128125</t>
+  </si>
+  <si>
+    <t>qimo2</t>
+  </si>
+  <si>
+    <t>sz128090</t>
+  </si>
+  <si>
+    <t>fenglong</t>
+  </si>
+  <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>tefa2</t>
+  </si>
+  <si>
+    <t>sz127021</t>
+  </si>
+  <si>
+    <t>xingsen</t>
+  </si>
+  <si>
+    <t>sz128122</t>
+  </si>
+  <si>
+    <t>punai</t>
+  </si>
+  <si>
+    <t>sz127035</t>
+  </si>
+  <si>
+    <t>lvyin</t>
+  </si>
+  <si>
+    <t>sz127034</t>
+  </si>
+  <si>
+    <t>lege</t>
+  </si>
+  <si>
+    <t>sz123072</t>
+  </si>
+  <si>
+    <t>beisi</t>
+  </si>
+  <si>
+    <t>sz123075</t>
+  </si>
+  <si>
+    <t>sannuo</t>
+  </si>
+  <si>
+    <t>sz123090</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ouzu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>s</t>
     </r>
     <r>
@@ -336,130 +536,258 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>123104</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123076</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123126</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128142</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lepu2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>xianglu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z128074</t>
+    </r>
+  </si>
+  <si>
+    <t>hugong</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h113593</t>
+    </r>
+  </si>
+  <si>
+    <t>peidi</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z123133</t>
+    </r>
+  </si>
+  <si>
+    <t>lingkang</t>
+  </si>
+  <si>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>zhongda</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>127048</t>
+    </r>
+  </si>
+  <si>
+    <t>weige</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>113527</t>
+    </r>
+  </si>
+  <si>
+    <t>leidi</t>
+  </si>
+  <si>
+    <t>sz123045</t>
+  </si>
+  <si>
+    <t>liande</t>
+  </si>
+  <si>
+    <t>sz123038</t>
+  </si>
+  <si>
+    <t>jufei</t>
+  </si>
+  <si>
+    <t>sz123050</t>
+  </si>
+  <si>
+    <t>puli</t>
+  </si>
+  <si>
+    <t>sz123099</t>
+  </si>
+  <si>
+    <t>xiongdi</t>
+  </si>
+  <si>
+    <t>sz128021</t>
+  </si>
+  <si>
+    <t>tai21</t>
+  </si>
+  <si>
+    <t>sh113638</t>
+  </si>
+  <si>
+    <t>fuhan</t>
+  </si>
+  <si>
+    <t>sz123122</t>
+  </si>
+  <si>
+    <t>chenfeng</t>
+  </si>
+  <si>
+    <t>sh113628</t>
+  </si>
+  <si>
+    <t>jiudian</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z123110</t>
+    </r>
+  </si>
+  <si>
+    <t>beilu</t>
+  </si>
+  <si>
+    <t>sz123082</t>
   </si>
   <si>
     <t>ruida</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>daoen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sz128116</t>
+  </si>
+  <si>
+    <t>huazheng</t>
+  </si>
+  <si>
+    <t>sh113639</t>
+  </si>
+  <si>
+    <t>chunzhong</t>
+  </si>
+  <si>
+    <t>sh113594</t>
+  </si>
+  <si>
+    <t>zongheng</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">128116 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2026/06/28</t>
   </si>
   <si>
     <t>jinbo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>xianggang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>huati</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123108</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>128072</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">128116 </t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2026/06/28</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>128117</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>sh</t>
     </r>
     <r>
@@ -467,356 +795,31 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">118001 </t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>113566</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh113574</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128125</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128090</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qimo2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>huayang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fenglong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128143</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz127021</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tefa2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128122</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>xingsen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz127035</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>punai</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz127034</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lvyin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lege</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123072</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>beisi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123075</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sannuo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123090</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ouzu</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z128074</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>h113593</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hugong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z123133</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>peidi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lingkang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhongda</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>weige</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>leidi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>liande</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>jufei</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>puli</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>xiongdi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tai21</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuhan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>chenfeng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh113610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>127048</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>sh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>113527</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123045</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123038</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123050</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>jiudian</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z123110</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123099</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128021</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh113638</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123122</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh113628</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>beilu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz123082</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruida</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sz128116</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>huazheng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh113639</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,12 +831,97 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -841,27 +929,250 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -884,32 +1195,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -958,7 +1555,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -993,7 +1590,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1196,60 +1793,60 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52:E52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
-    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3727272727273" customWidth="1"/>
+    <col min="9" max="9" width="11.6272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2">
@@ -1265,7 +1862,7 @@
         <v>1.8</v>
       </c>
       <c r="G2">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="H2">
         <v>15</v>
@@ -1274,11 +1871,11 @@
         <v>46016</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3">
@@ -1303,11 +1900,11 @@
         <v>46224</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C4">
@@ -1332,11 +1929,11 @@
         <v>46405</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C5">
@@ -1361,11 +1958,11 @@
         <v>46196</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6">
@@ -1390,11 +1987,11 @@
         <v>45832</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C7">
@@ -1419,11 +2016,11 @@
         <v>46560</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C8">
@@ -1448,11 +2045,11 @@
         <v>46268</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C9">
@@ -1477,11 +2074,11 @@
         <v>45491</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -1506,11 +2103,11 @@
         <v>46092</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11">
@@ -1535,11 +2132,11 @@
         <v>46349</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C12">
@@ -1564,11 +2161,11 @@
         <v>46412</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C13">
@@ -1593,11 +2190,11 @@
         <v>45736</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C14">
@@ -1622,12 +2219,12 @@
         <v>46124</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C15">
         <v>0.3</v>
@@ -1651,12 +2248,12 @@
         <v>46461</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>41</v>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -1680,12 +2277,12 @@
         <v>46344</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>42</v>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C17">
         <v>0.5</v>
@@ -1709,12 +2306,12 @@
         <v>46639</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>43</v>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C18">
         <v>0.4</v>
@@ -1738,11 +2335,11 @@
         <v>46469</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C19">
@@ -1767,12 +2364,12 @@
         <v>46373</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C20">
         <v>0.4</v>
@@ -1796,12 +2393,12 @@
         <v>46204</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C21">
         <v>0.5</v>
@@ -1816,7 +2413,7 @@
         <v>1.8</v>
       </c>
       <c r="G21">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H21">
         <v>18</v>
@@ -1825,12 +2422,12 @@
         <v>46080</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C22">
         <v>0.5</v>
@@ -1845,7 +2442,7 @@
         <v>1.8</v>
       </c>
       <c r="G22">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -1854,12 +2451,12 @@
         <v>46111</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C23">
         <v>0.4</v>
@@ -1883,12 +2480,12 @@
         <v>45888</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1912,12 +2509,12 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C25">
         <v>0.4</v>
@@ -1937,16 +2534,16 @@
       <c r="H25">
         <v>13</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="6">
         <v>46232</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C26">
         <v>0.3</v>
@@ -1970,12 +2567,12 @@
         <v>46017</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C27">
         <v>0.5</v>
@@ -1999,12 +2596,12 @@
         <v>46394</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2028,12 +2625,12 @@
         <v>45875</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2057,12 +2654,12 @@
         <v>45860</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2080,18 +2677,18 @@
         <v>3</v>
       </c>
       <c r="H30">
-        <v>8.8000000000000007</v>
+        <v>8.8</v>
       </c>
       <c r="I30" s="3">
         <v>46167</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C31">
         <v>0.4</v>
@@ -2115,12 +2712,12 @@
         <v>46506</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C32">
         <v>0.5</v>
@@ -2144,12 +2741,12 @@
         <v>46315</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C33">
         <v>0.4</v>
@@ -2173,12 +2770,12 @@
         <v>46327</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C34">
         <v>0.3</v>
@@ -2202,12 +2799,12 @@
         <v>46376</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>81</v>
+    <row r="35" spans="1:9">
+      <c r="A35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C35">
         <v>0.4</v>
@@ -2231,12 +2828,12 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>82</v>
+    <row r="36" spans="1:9">
+      <c r="A36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C36">
         <v>0.4</v>
@@ -2260,12 +2857,12 @@
         <v>46222</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>84</v>
+    <row r="37" spans="1:9">
+      <c r="A37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="C37">
         <v>0.4</v>
@@ -2289,12 +2886,12 @@
         <v>46742</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>97</v>
+    <row r="38" spans="1:9">
+      <c r="A38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C38">
         <v>0.4</v>
@@ -2318,12 +2915,12 @@
         <v>46356</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>98</v>
+    <row r="39" spans="1:9">
+      <c r="A39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C39">
         <v>0.4</v>
@@ -2347,12 +2944,12 @@
         <v>46685</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>99</v>
+    <row r="40" spans="1:9">
+      <c r="A40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C40">
         <v>0.5</v>
@@ -2376,12 +2973,12 @@
         <v>45680</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>100</v>
+    <row r="41" spans="1:9">
+      <c r="A41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C41">
         <v>0.5</v>
@@ -2396,7 +2993,7 @@
         <v>1.8</v>
       </c>
       <c r="G41">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H41">
         <v>13</v>
@@ -2405,12 +3002,12 @@
         <v>46092</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:9">
+      <c r="A42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="C42">
         <v>0.5</v>
@@ -2419,7 +3016,7 @@
         <v>0.7</v>
       </c>
       <c r="E42">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="F42">
         <v>1.7</v>
@@ -2434,12 +3031,12 @@
         <v>46015</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:9">
+      <c r="A43" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>102</v>
+      <c r="B43" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C43">
         <v>0.4</v>
@@ -2463,12 +3060,12 @@
         <v>46125</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A44" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>105</v>
+    <row r="44" spans="1:9">
+      <c r="A44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C44">
         <v>0.4</v>
@@ -2492,12 +3089,12 @@
         <v>46426</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A45" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>106</v>
+    <row r="45" spans="1:9">
+      <c r="A45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C45">
         <v>0.3</v>
@@ -2521,12 +3118,12 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A46" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>107</v>
+    <row r="46" spans="1:9">
+      <c r="A46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C46">
         <v>0.3</v>
@@ -2550,12 +3147,12 @@
         <v>46749</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A47" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>108</v>
+    <row r="47" spans="1:9">
+      <c r="A47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="C47">
         <v>0.3</v>
@@ -2579,12 +3176,12 @@
         <v>46604</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>109</v>
+    <row r="48" spans="1:9">
+      <c r="A48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C48">
         <v>0.5</v>
@@ -2608,11 +3205,11 @@
         <v>46621</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:9">
+      <c r="A49" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C49">
@@ -2637,12 +3234,12 @@
         <v>46477</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A50" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>111</v>
+    <row r="50" spans="1:9">
+      <c r="A50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -2666,12 +3263,12 @@
         <v>46362</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A51" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>113</v>
+    <row r="51" spans="1:9">
+      <c r="A51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C51">
         <v>0.4</v>
@@ -2695,12 +3292,12 @@
         <v>46201</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>115</v>
+    <row r="52" spans="1:9">
+      <c r="A52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C52">
         <v>0.2</v>
@@ -2724,32 +3321,91 @@
         <v>46775</v>
       </c>
     </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53">
+        <v>0.5</v>
+      </c>
+      <c r="D53">
+        <v>0.7</v>
+      </c>
+      <c r="E53">
+        <v>1.2</v>
+      </c>
+      <c r="F53">
+        <v>1.8</v>
+      </c>
+      <c r="G53">
+        <v>2.2</v>
+      </c>
+      <c r="H53">
+        <v>15</v>
+      </c>
+      <c r="I53" s="3">
+        <v>46223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54">
+        <v>0.5</v>
+      </c>
+      <c r="D54">
+        <v>0.7</v>
+      </c>
+      <c r="E54">
+        <v>1.2</v>
+      </c>
+      <c r="F54">
+        <v>1.8</v>
+      </c>
+      <c r="G54">
+        <v>2.5</v>
+      </c>
+      <c r="H54">
+        <v>18</v>
+      </c>
+      <c r="I54" s="3">
+        <v>46128</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I2"/>
+      <selection activeCell="A1" sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C1">
         <v>0.4</v>
@@ -2769,16 +3425,16 @@
       <c r="H1">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I1" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>117</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -2803,7 +3459,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1.update dafeng to interest.xlsx and readme
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>name</t>
   </si>
@@ -750,6 +750,18 @@
   </si>
   <si>
     <t>sh113573</t>
+  </si>
+  <si>
+    <t>wanxing</t>
+  </si>
+  <si>
+    <t>sz123116</t>
+  </si>
+  <si>
+    <t>dafeng</t>
+  </si>
+  <si>
+    <t>sh113530</t>
   </si>
   <si>
     <r>
@@ -807,19 +819,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -835,7 +840,59 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,8 +906,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -865,109 +970,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -987,7 +992,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -999,7 +1016,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,7 +1058,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,7 +1094,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1041,127 +1166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,13 +1201,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1216,17 +1240,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1264,32 +1282,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1299,10 +1304,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1311,146 +1316,145 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1799,10 +1803,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:I54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2534,7 +2538,7 @@
       <c r="H25">
         <v>13</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>46232</v>
       </c>
     </row>
@@ -2948,7 +2952,7 @@
       <c r="A40" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C40">
@@ -2977,7 +2981,7 @@
       <c r="A41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C41">
@@ -3006,7 +3010,7 @@
       <c r="A42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42">
@@ -3035,7 +3039,7 @@
       <c r="A43" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C43">
@@ -3064,7 +3068,7 @@
       <c r="A44" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C44">
@@ -3093,7 +3097,7 @@
       <c r="A45" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C45">
@@ -3122,7 +3126,7 @@
       <c r="A46" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C46">
@@ -3151,7 +3155,7 @@
       <c r="A47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C47">
@@ -3180,7 +3184,7 @@
       <c r="A48" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C48">
@@ -3377,6 +3381,64 @@
       </c>
       <c r="I54" s="3">
         <v>46128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55">
+        <v>0.4</v>
+      </c>
+      <c r="D55">
+        <v>0.7</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1.8</v>
+      </c>
+      <c r="G55">
+        <v>2.5</v>
+      </c>
+      <c r="H55">
+        <v>15</v>
+      </c>
+      <c r="I55" s="3">
+        <v>46546</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56">
+        <v>0.4</v>
+      </c>
+      <c r="D56">
+        <v>0.6</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1.5</v>
+      </c>
+      <c r="G56">
+        <v>2.5</v>
+      </c>
+      <c r="H56">
+        <v>16</v>
+      </c>
+      <c r="I56" s="3">
+        <v>45011</v>
       </c>
     </row>
   </sheetData>
@@ -3405,7 +3467,7 @@
         <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C1">
         <v>0.4</v>
@@ -3426,15 +3488,15 @@
         <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C2">
         <v>0.5</v>

</xml_diff>

<commit_message>
1.get advised by ka shen
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7270"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -262,12 +262,6 @@
     <t>sz123096</t>
   </si>
   <si>
-    <t>disen</t>
-  </si>
-  <si>
-    <t>sz123023</t>
-  </si>
-  <si>
     <t>weier</t>
   </si>
   <si>
@@ -649,12 +643,6 @@
     </r>
   </si>
   <si>
-    <t>leidi</t>
-  </si>
-  <si>
-    <t>sz123045</t>
-  </si>
-  <si>
     <t>liande</t>
   </si>
   <si>
@@ -762,6 +750,18 @@
   </si>
   <si>
     <t>sh113530</t>
+  </si>
+  <si>
+    <t>jiali</t>
+  </si>
+  <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>huayuan</t>
+  </si>
+  <si>
+    <t>sz128049</t>
   </si>
   <si>
     <r>
@@ -1805,8 +1805,8 @@
   <sheetPr/>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2173,25 +2173,25 @@
         <v>32</v>
       </c>
       <c r="C13">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D13">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F13">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G13">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="H13">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I13" s="3">
-        <v>45736</v>
+        <v>46124</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2202,25 +2202,25 @@
         <v>34</v>
       </c>
       <c r="C14">
+        <v>0.3</v>
+      </c>
+      <c r="D14">
         <v>0.5</v>
       </c>
-      <c r="D14">
-        <v>0.8</v>
-      </c>
       <c r="E14">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F14">
+        <v>1.5</v>
+      </c>
+      <c r="G14">
         <v>1.8</v>
       </c>
-      <c r="G14">
-        <v>2.5</v>
-      </c>
       <c r="H14">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="3">
-        <v>46124</v>
+        <v>46461</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2231,10 +2231,10 @@
         <v>36</v>
       </c>
       <c r="C15">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D15">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -2243,13 +2243,13 @@
         <v>1.5</v>
       </c>
       <c r="G15">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I15" s="3">
-        <v>46461</v>
+        <v>46344</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2260,25 +2260,25 @@
         <v>38</v>
       </c>
       <c r="C16">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D16">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="F16">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H16">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I16" s="3">
-        <v>46344</v>
+        <v>46639</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2289,25 +2289,25 @@
         <v>40</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E17">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G17">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>20</v>
       </c>
       <c r="I17" s="3">
-        <v>46639</v>
+        <v>46469</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2318,10 +2318,10 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D18">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2330,27 +2330,27 @@
         <v>1.5</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H18">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I18" s="3">
-        <v>46469</v>
+        <v>46373</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C19">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -2359,13 +2359,13 @@
         <v>1.5</v>
       </c>
       <c r="G19">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="H19">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I19" s="3">
-        <v>46373</v>
+        <v>46204</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2376,25 +2376,25 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D20">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F20">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="H20">
         <v>18</v>
       </c>
       <c r="I20" s="3">
-        <v>46204</v>
+        <v>46080</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2408,7 +2408,7 @@
         <v>0.5</v>
       </c>
       <c r="D21">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E21">
         <v>1.2</v>
@@ -2420,10 +2420,10 @@
         <v>2.2</v>
       </c>
       <c r="H21">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I21" s="3">
-        <v>46080</v>
+        <v>46111</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2434,25 +2434,25 @@
         <v>50</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="E22">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G22">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22" s="3">
-        <v>46111</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2463,25 +2463,25 @@
         <v>52</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
         <v>1.5</v>
       </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
       <c r="H23">
-        <v>10</v>
+        <v>7.8</v>
       </c>
       <c r="I23" s="3">
-        <v>45888</v>
+        <v>46110</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2492,25 +2492,25 @@
         <v>54</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D24">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="E24">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G24">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>7.8</v>
-      </c>
-      <c r="I24" s="3">
-        <v>46110</v>
+        <v>13</v>
+      </c>
+      <c r="I24" s="5">
+        <v>46232</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2521,7 +2521,7 @@
         <v>56</v>
       </c>
       <c r="C25">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D25">
         <v>0.6</v>
@@ -2533,13 +2533,13 @@
         <v>1.5</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H25">
-        <v>13</v>
-      </c>
-      <c r="I25" s="5">
-        <v>46232</v>
+        <v>10</v>
+      </c>
+      <c r="I25" s="3">
+        <v>46017</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2550,25 +2550,25 @@
         <v>58</v>
       </c>
       <c r="C26">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D26">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F26">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G26">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="H26">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I26" s="3">
-        <v>46017</v>
+        <v>46394</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2579,25 +2579,25 @@
         <v>60</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.3</v>
+      </c>
+      <c r="E27">
         <v>0.5</v>
       </c>
-      <c r="D27">
-        <v>0.7</v>
-      </c>
-      <c r="E27">
-        <v>1.2</v>
-      </c>
       <c r="F27">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="H27">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I27" s="3">
-        <v>46394</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2626,7 +2626,7 @@
         <v>10</v>
       </c>
       <c r="I28" s="3">
-        <v>45875</v>
+        <v>45860</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2640,22 +2640,22 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="E29">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G29">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>8.8</v>
       </c>
       <c r="I29" s="3">
-        <v>45860</v>
+        <v>46167</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2666,25 +2666,25 @@
         <v>66</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D30">
         <v>0.6</v>
       </c>
       <c r="E30">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>1.5</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H30">
-        <v>8.8</v>
+        <v>13</v>
       </c>
       <c r="I30" s="3">
-        <v>46167</v>
+        <v>46506</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2695,25 +2695,25 @@
         <v>68</v>
       </c>
       <c r="C31">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D31">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="F31">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G31">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="H31">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I31" s="3">
-        <v>46506</v>
+        <v>46315</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2724,25 +2724,25 @@
         <v>70</v>
       </c>
       <c r="C32">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D32">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E32">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G32">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="H32">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I32" s="3">
-        <v>46315</v>
+        <v>46327</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2753,10 +2753,10 @@
         <v>72</v>
       </c>
       <c r="C33">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D33">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2765,27 +2765,27 @@
         <v>1.5</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H33">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I33" s="3">
-        <v>46327</v>
+        <v>46376</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C34">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D34">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -2797,10 +2797,10 @@
         <v>1.8</v>
       </c>
       <c r="H34">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I34" s="3">
-        <v>46376</v>
+        <v>45922</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2817,19 +2817,19 @@
         <v>0.6</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F35">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="H35">
         <v>15</v>
       </c>
       <c r="I35" s="3">
-        <v>45922</v>
+        <v>46222</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2846,19 +2846,19 @@
         <v>0.6</v>
       </c>
       <c r="E36">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F36">
+        <v>1.5</v>
+      </c>
+      <c r="G36">
         <v>2</v>
-      </c>
-      <c r="G36">
-        <v>2.4</v>
       </c>
       <c r="H36">
         <v>15</v>
       </c>
       <c r="I36" s="3">
-        <v>46222</v>
+        <v>46742</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2872,7 +2872,7 @@
         <v>0.4</v>
       </c>
       <c r="D37">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2881,13 +2881,13 @@
         <v>1.5</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H37">
         <v>15</v>
       </c>
       <c r="I37" s="3">
-        <v>46742</v>
+        <v>46356</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2901,13 +2901,13 @@
         <v>0.4</v>
       </c>
       <c r="D38">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F38">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G38">
         <v>2.5</v>
@@ -2916,7 +2916,7 @@
         <v>15</v>
       </c>
       <c r="I38" s="3">
-        <v>46356</v>
+        <v>46685</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2927,25 +2927,25 @@
         <v>84</v>
       </c>
       <c r="C39">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D39">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E39">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G39">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>15</v>
       </c>
       <c r="I39" s="3">
-        <v>46685</v>
+        <v>45680</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2962,19 +2962,19 @@
         <v>0.7</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="F40">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="H40">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I40" s="3">
-        <v>45680</v>
+        <v>46015</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2985,25 +2985,25 @@
         <v>88</v>
       </c>
       <c r="C41">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D41">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E41">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G41">
-        <v>2.2</v>
+        <v>2.5</v>
       </c>
       <c r="H41">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I41" s="3">
-        <v>46092</v>
+        <v>46125</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3014,25 +3014,25 @@
         <v>90</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D42">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="E42">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="G42">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="H42">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I42" s="3">
-        <v>46015</v>
+        <v>46426</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3043,25 +3043,25 @@
         <v>92</v>
       </c>
       <c r="C43">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D43">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
+        <v>1.3</v>
+      </c>
+      <c r="G43">
         <v>1.5</v>
       </c>
-      <c r="G43">
-        <v>2.5</v>
-      </c>
       <c r="H43">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I43" s="3">
-        <v>46125</v>
+        <v>45257</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3072,10 +3072,10 @@
         <v>94</v>
       </c>
       <c r="C44">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D44">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -3084,13 +3084,13 @@
         <v>1.5</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H44">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I44" s="3">
-        <v>46426</v>
+        <v>46749</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3110,16 +3110,16 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="G45">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H45">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I45" s="3">
-        <v>45257</v>
+        <v>46604</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3130,61 +3130,61 @@
         <v>98</v>
       </c>
       <c r="C46">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D46">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G46">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="H46">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I46" s="3">
-        <v>46749</v>
+        <v>46621</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C47">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D47">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F47">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="H47">
         <v>15</v>
       </c>
       <c r="I47" s="3">
-        <v>46604</v>
+        <v>46477</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C48">
@@ -3194,10 +3194,10 @@
         <v>0.7</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="G48">
         <v>2.5</v>
@@ -3206,7 +3206,7 @@
         <v>15</v>
       </c>
       <c r="I48" s="3">
-        <v>46621</v>
+        <v>46362</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3220,22 +3220,22 @@
         <v>0.4</v>
       </c>
       <c r="D49">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E49">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G49">
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="H49">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I49" s="3">
-        <v>46477</v>
+        <v>46201</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3246,83 +3246,83 @@
         <v>106</v>
       </c>
       <c r="C50">
+        <v>0.2</v>
+      </c>
+      <c r="D50">
+        <v>0.4</v>
+      </c>
+      <c r="E50">
+        <v>0.6</v>
+      </c>
+      <c r="F50">
+        <v>1.5</v>
+      </c>
+      <c r="G50">
+        <v>1.8</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
+      </c>
+      <c r="I50" s="3">
+        <v>46775</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51">
         <v>0.5</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>0.7</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>1.2</v>
       </c>
-      <c r="F50">
+      <c r="F51">
         <v>1.8</v>
       </c>
-      <c r="G50">
+      <c r="G51">
+        <v>2.2</v>
+      </c>
+      <c r="H51">
+        <v>15</v>
+      </c>
+      <c r="I51" s="3">
+        <v>46223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52">
+        <v>0.5</v>
+      </c>
+      <c r="D52">
+        <v>0.7</v>
+      </c>
+      <c r="E52">
+        <v>1.2</v>
+      </c>
+      <c r="F52">
+        <v>1.8</v>
+      </c>
+      <c r="G52">
         <v>2.5</v>
       </c>
-      <c r="H50">
-        <v>15</v>
-      </c>
-      <c r="I50" s="3">
-        <v>46362</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51">
-        <v>0.4</v>
-      </c>
-      <c r="D51">
-        <v>0.5</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
-        <v>1.5</v>
-      </c>
-      <c r="G51">
-        <v>1.9</v>
-      </c>
-      <c r="H51">
-        <v>10</v>
-      </c>
-      <c r="I51" s="3">
-        <v>46201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52">
-        <v>0.2</v>
-      </c>
-      <c r="D52">
-        <v>0.4</v>
-      </c>
-      <c r="E52">
-        <v>0.6</v>
-      </c>
-      <c r="F52">
-        <v>1.5</v>
-      </c>
-      <c r="G52">
-        <v>1.8</v>
-      </c>
       <c r="H52">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I52" s="3">
-        <v>46775</v>
+        <v>46128</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3333,25 +3333,25 @@
         <v>112</v>
       </c>
       <c r="C53">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D53">
         <v>0.7</v>
       </c>
       <c r="E53">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F53">
         <v>1.8</v>
       </c>
       <c r="G53">
-        <v>2.2</v>
+        <v>2.5</v>
       </c>
       <c r="H53">
         <v>15</v>
       </c>
       <c r="I53" s="3">
-        <v>46223</v>
+        <v>46546</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3362,25 +3362,25 @@
         <v>114</v>
       </c>
       <c r="C54">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D54">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="E54">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F54">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G54">
         <v>2.5</v>
       </c>
       <c r="H54">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I54" s="3">
-        <v>46128</v>
+        <v>45011</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3391,7 +3391,7 @@
         <v>116</v>
       </c>
       <c r="C55">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D55">
         <v>0.7</v>
@@ -3406,10 +3406,10 @@
         <v>2.5</v>
       </c>
       <c r="H55">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I55" s="3">
-        <v>46546</v>
+        <v>46232</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3420,10 +3420,10 @@
         <v>118</v>
       </c>
       <c r="C56">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D56">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3432,13 +3432,13 @@
         <v>1.5</v>
       </c>
       <c r="G56">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H56">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I56" s="3">
-        <v>45011</v>
+        <v>45622</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3464,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
1.add some items in interest.xlsx 2.fix bug in cartridge about trade years
</commit_message>
<xml_diff>
--- a/interest.xlsx
+++ b/interest.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="bad" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
   <si>
     <t>name</t>
   </si>
@@ -764,6 +764,114 @@
     <t>sz128049</t>
   </si>
   <si>
+    <t>tuosi</t>
+  </si>
+  <si>
+    <t>sz123101</t>
+  </si>
+  <si>
+    <t>aofei</t>
+  </si>
+  <si>
+    <t>sz123131</t>
+  </si>
+  <si>
+    <t>zhonglu</t>
+  </si>
+  <si>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>weipai</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>fengyu</t>
+  </si>
+  <si>
+    <t>sh113643</t>
+  </si>
+  <si>
+    <t>langke</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>jinji</t>
+  </si>
+  <si>
+    <t>sz123129</t>
+  </si>
+  <si>
+    <t>kangyi</t>
+  </si>
+  <si>
+    <t>sz123151</t>
+  </si>
+  <si>
+    <t>silu</t>
+  </si>
+  <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>bohui</t>
+  </si>
+  <si>
+    <t>sz123156</t>
+  </si>
+  <si>
+    <t>naipu</t>
+  </si>
+  <si>
+    <t>sz123127</t>
+  </si>
+  <si>
+    <t>aojia</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>bojie</t>
+  </si>
+  <si>
+    <t>sz127051</t>
+  </si>
+  <si>
+    <t>guoguang</t>
+  </si>
+  <si>
+    <t>sz128123</t>
+  </si>
+  <si>
+    <t>leizhi</t>
+  </si>
+  <si>
+    <t>sz127062</t>
+  </si>
+  <si>
+    <t>dibei</t>
+  </si>
+  <si>
+    <t>sh113546</t>
+  </si>
+  <si>
+    <t>linggang</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>rongtai</t>
+  </si>
+  <si>
+    <t>sh113606</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -812,6 +920,12 @@
       </rPr>
       <t xml:space="preserve">118001 </t>
     </r>
+  </si>
+  <si>
+    <t>boshi</t>
+  </si>
+  <si>
+    <t>sz127072</t>
   </si>
 </sst>
 </file>
@@ -983,12 +1097,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1304,10 +1424,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1316,16 +1436,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1337,10 +1457,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1361,28 +1481,28 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1391,19 +1511,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1415,42 +1532,47 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1803,10 +1925,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1817,34 +1939,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -1871,7 +1993,7 @@
       <c r="H2">
         <v>15</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>46016</v>
       </c>
     </row>
@@ -1900,7 +2022,7 @@
       <c r="H3">
         <v>18</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
         <v>46224</v>
       </c>
     </row>
@@ -1929,7 +2051,7 @@
       <c r="H4">
         <v>24</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="4">
         <v>46405</v>
       </c>
     </row>
@@ -1958,7 +2080,7 @@
       <c r="H5">
         <v>15</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
         <v>46196</v>
       </c>
     </row>
@@ -1987,7 +2109,7 @@
       <c r="H6">
         <v>15</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <v>45832</v>
       </c>
     </row>
@@ -2016,7 +2138,7 @@
       <c r="H7">
         <v>10</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="4">
         <v>46560</v>
       </c>
     </row>
@@ -2045,7 +2167,7 @@
       <c r="H8">
         <v>15</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="4">
         <v>46268</v>
       </c>
     </row>
@@ -2074,7 +2196,7 @@
       <c r="H9">
         <v>14</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <v>45491</v>
       </c>
     </row>
@@ -2103,7 +2225,7 @@
       <c r="H10">
         <v>21.5</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="4">
         <v>46092</v>
       </c>
     </row>
@@ -2132,7 +2254,7 @@
       <c r="H11">
         <v>18</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="4">
         <v>46349</v>
       </c>
     </row>
@@ -2161,7 +2283,7 @@
       <c r="H12">
         <v>21</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="4">
         <v>46412</v>
       </c>
     </row>
@@ -2190,7 +2312,7 @@
       <c r="H13">
         <v>21</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="4">
         <v>46124</v>
       </c>
     </row>
@@ -2219,7 +2341,7 @@
       <c r="H14">
         <v>20</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="4">
         <v>46461</v>
       </c>
     </row>
@@ -2248,7 +2370,7 @@
       <c r="H15">
         <v>13</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="4">
         <v>46344</v>
       </c>
     </row>
@@ -2277,7 +2399,7 @@
       <c r="H16">
         <v>20</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="4">
         <v>46639</v>
       </c>
     </row>
@@ -2306,7 +2428,7 @@
       <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="4">
         <v>46469</v>
       </c>
     </row>
@@ -2335,7 +2457,7 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="4">
         <v>46373</v>
       </c>
     </row>
@@ -2364,7 +2486,7 @@
       <c r="H19">
         <v>18</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="4">
         <v>46204</v>
       </c>
     </row>
@@ -2393,7 +2515,7 @@
       <c r="H20">
         <v>18</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="4">
         <v>46080</v>
       </c>
     </row>
@@ -2422,7 +2544,7 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="4">
         <v>46111</v>
       </c>
     </row>
@@ -2451,7 +2573,7 @@
       <c r="H22">
         <v>10</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="4">
         <v>45888</v>
       </c>
     </row>
@@ -2480,7 +2602,7 @@
       <c r="H23">
         <v>7.8</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="4">
         <v>46110</v>
       </c>
     </row>
@@ -2509,7 +2631,7 @@
       <c r="H24">
         <v>13</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="7">
         <v>46232</v>
       </c>
     </row>
@@ -2538,7 +2660,7 @@
       <c r="H25">
         <v>10</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="4">
         <v>46017</v>
       </c>
     </row>
@@ -2567,7 +2689,7 @@
       <c r="H26">
         <v>15</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="4">
         <v>46394</v>
       </c>
     </row>
@@ -2596,7 +2718,7 @@
       <c r="H27">
         <v>10</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="4">
         <v>45875</v>
       </c>
     </row>
@@ -2625,7 +2747,7 @@
       <c r="H28">
         <v>10</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="4">
         <v>45860</v>
       </c>
     </row>
@@ -2654,7 +2776,7 @@
       <c r="H29">
         <v>8.8</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="4">
         <v>46167</v>
       </c>
     </row>
@@ -2683,7 +2805,7 @@
       <c r="H30">
         <v>13</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="4">
         <v>46506</v>
       </c>
     </row>
@@ -2712,7 +2834,7 @@
       <c r="H31">
         <v>20</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="4">
         <v>46315</v>
       </c>
     </row>
@@ -2741,7 +2863,7 @@
       <c r="H32">
         <v>10</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="4">
         <v>46327</v>
       </c>
     </row>
@@ -2770,12 +2892,12 @@
       <c r="H33">
         <v>12</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="4">
         <v>46376</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2799,12 +2921,12 @@
       <c r="H34">
         <v>15</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="4">
         <v>45922</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2828,12 +2950,12 @@
       <c r="H35">
         <v>15</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="4">
         <v>46222</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2857,12 +2979,12 @@
       <c r="H36">
         <v>15</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="4">
         <v>46742</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2886,12 +3008,12 @@
       <c r="H37">
         <v>15</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="4">
         <v>46356</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2915,12 +3037,12 @@
       <c r="H38">
         <v>15</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="4">
         <v>46685</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2944,12 +3066,12 @@
       <c r="H39">
         <v>15</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="4">
         <v>45680</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2973,12 +3095,12 @@
       <c r="H40">
         <v>13</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="4">
         <v>46015</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3002,12 +3124,12 @@
       <c r="H41">
         <v>18</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="4">
         <v>46125</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3031,12 +3153,12 @@
       <c r="H42">
         <v>18</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="4">
         <v>46426</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3060,12 +3182,12 @@
       <c r="H43">
         <v>6</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="4">
         <v>45257</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3089,12 +3211,12 @@
       <c r="H44">
         <v>12</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="4">
         <v>46749</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3118,12 +3240,12 @@
       <c r="H45">
         <v>15</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="4">
         <v>46604</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -3147,15 +3269,15 @@
       <c r="H46">
         <v>15</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="4">
         <v>46621</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C47">
@@ -3176,15 +3298,15 @@
       <c r="H47">
         <v>15</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="4">
         <v>46477</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C48">
@@ -3205,15 +3327,15 @@
       <c r="H48">
         <v>15</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="4">
         <v>46362</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C49">
@@ -3234,15 +3356,15 @@
       <c r="H49">
         <v>10</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="4">
         <v>46201</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C50">
@@ -3263,7 +3385,7 @@
       <c r="H50">
         <v>8</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="4">
         <v>46775</v>
       </c>
     </row>
@@ -3292,7 +3414,7 @@
       <c r="H51">
         <v>15</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="4">
         <v>46223</v>
       </c>
     </row>
@@ -3321,7 +3443,7 @@
       <c r="H52">
         <v>18</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="4">
         <v>46128</v>
       </c>
     </row>
@@ -3350,7 +3472,7 @@
       <c r="H53">
         <v>15</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="4">
         <v>46546</v>
       </c>
     </row>
@@ -3379,7 +3501,7 @@
       <c r="H54">
         <v>16</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="4">
         <v>45011</v>
       </c>
     </row>
@@ -3408,7 +3530,7 @@
       <c r="H55">
         <v>18</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55" s="4">
         <v>46232</v>
       </c>
     </row>
@@ -3437,8 +3559,530 @@
       <c r="H56">
         <v>3</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="4">
         <v>45622</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57">
+        <v>0.3</v>
+      </c>
+      <c r="D57">
+        <v>0.5</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1.5</v>
+      </c>
+      <c r="G57">
+        <v>1.8</v>
+      </c>
+      <c r="H57">
+        <v>10</v>
+      </c>
+      <c r="I57" s="4">
+        <v>46455</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58">
+        <v>0.5</v>
+      </c>
+      <c r="D58">
+        <v>0.7</v>
+      </c>
+      <c r="E58">
+        <v>1.2</v>
+      </c>
+      <c r="F58">
+        <v>1.8</v>
+      </c>
+      <c r="G58">
+        <v>2.5</v>
+      </c>
+      <c r="H58">
+        <v>15</v>
+      </c>
+      <c r="I58" s="4">
+        <v>46723</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59">
+        <v>0.4</v>
+      </c>
+      <c r="D59">
+        <v>0.6</v>
+      </c>
+      <c r="E59">
+        <v>1.2</v>
+      </c>
+      <c r="F59">
+        <v>1.8</v>
+      </c>
+      <c r="G59">
+        <v>2.5</v>
+      </c>
+      <c r="H59">
+        <v>15</v>
+      </c>
+      <c r="I59" s="4">
+        <v>46976</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60">
+        <v>0.5</v>
+      </c>
+      <c r="D60">
+        <v>0.7</v>
+      </c>
+      <c r="E60">
+        <v>1.2</v>
+      </c>
+      <c r="F60">
+        <v>1.8</v>
+      </c>
+      <c r="G60">
+        <v>2.4</v>
+      </c>
+      <c r="H60">
+        <v>15</v>
+      </c>
+      <c r="I60" s="4">
+        <v>46334</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61">
+        <v>0.3</v>
+      </c>
+      <c r="D61">
+        <v>0.5</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1.5</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>15</v>
+      </c>
+      <c r="I61" s="4">
+        <v>46836</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62">
+        <v>0.4</v>
+      </c>
+      <c r="D62">
+        <v>0.6</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1.5</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>12</v>
+      </c>
+      <c r="I62" s="4">
+        <v>46426</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63">
+        <v>0.4</v>
+      </c>
+      <c r="D63">
+        <v>0.6</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1.5</v>
+      </c>
+      <c r="G63">
+        <v>2.3</v>
+      </c>
+      <c r="H63">
+        <v>12</v>
+      </c>
+      <c r="I63" s="4">
+        <v>46694</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64">
+        <v>0.4</v>
+      </c>
+      <c r="D64">
+        <v>0.7</v>
+      </c>
+      <c r="E64">
+        <v>1.2</v>
+      </c>
+      <c r="F64">
+        <v>1.8</v>
+      </c>
+      <c r="G64">
+        <v>2.5</v>
+      </c>
+      <c r="H64">
+        <v>15</v>
+      </c>
+      <c r="I64" s="4">
+        <v>46934</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65">
+        <v>0.5</v>
+      </c>
+      <c r="D65">
+        <v>0.7</v>
+      </c>
+      <c r="E65">
+        <v>1.2</v>
+      </c>
+      <c r="F65">
+        <v>1.8</v>
+      </c>
+      <c r="G65">
+        <v>2.5</v>
+      </c>
+      <c r="H65">
+        <v>15</v>
+      </c>
+      <c r="I65" s="4">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66">
+        <v>0.4</v>
+      </c>
+      <c r="D66">
+        <v>0.6</v>
+      </c>
+      <c r="E66">
+        <v>1.1</v>
+      </c>
+      <c r="F66">
+        <v>1.8</v>
+      </c>
+      <c r="G66">
+        <v>2.4</v>
+      </c>
+      <c r="H66">
+        <v>15</v>
+      </c>
+      <c r="I66" s="4">
+        <v>46980</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67">
+        <v>0.4</v>
+      </c>
+      <c r="D67">
+        <v>0.6</v>
+      </c>
+      <c r="E67">
+        <v>1.1</v>
+      </c>
+      <c r="F67">
+        <v>1.8</v>
+      </c>
+      <c r="G67">
+        <v>2.3</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67" s="4">
+        <v>46688</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68">
+        <v>0.4</v>
+      </c>
+      <c r="D68">
+        <v>0.6</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1.5</v>
+      </c>
+      <c r="G68">
+        <v>1.8</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68" s="4">
+        <v>46077</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69">
+        <v>0.4</v>
+      </c>
+      <c r="D69">
+        <v>0.6</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1.6</v>
+      </c>
+      <c r="G69">
+        <v>2.5</v>
+      </c>
+      <c r="H69">
+        <v>15</v>
+      </c>
+      <c r="I69" s="4">
+        <v>46707</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70">
+        <v>0.5</v>
+      </c>
+      <c r="D70">
+        <v>0.7</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1.5</v>
+      </c>
+      <c r="G70">
+        <v>2.5</v>
+      </c>
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70" s="4">
+        <v>46229</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71">
+        <v>0.4</v>
+      </c>
+      <c r="D71">
+        <v>0.6</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1.5</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <v>15</v>
+      </c>
+      <c r="I71" s="4">
+        <v>46863</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72">
+        <v>0.5</v>
+      </c>
+      <c r="D72">
+        <v>0.8</v>
+      </c>
+      <c r="E72">
+        <v>1.2</v>
+      </c>
+      <c r="F72">
+        <v>1.6</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>15</v>
+      </c>
+      <c r="I72" s="4">
+        <v>45952</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73">
+        <v>0.4</v>
+      </c>
+      <c r="D73">
+        <v>0.7</v>
+      </c>
+      <c r="E73">
+        <v>1.1</v>
+      </c>
+      <c r="F73">
+        <v>1.6</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73">
+        <v>12</v>
+      </c>
+      <c r="I73" s="4">
+        <v>46124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74">
+        <v>0.5</v>
+      </c>
+      <c r="D74">
+        <v>0.7</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1.5</v>
+      </c>
+      <c r="G74">
+        <v>2.5</v>
+      </c>
+      <c r="H74">
+        <v>15</v>
+      </c>
+      <c r="I74" s="4">
+        <v>46324</v>
       </c>
     </row>
   </sheetData>
@@ -3451,13 +4095,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I2"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
   <cols>
     <col min="9" max="9" width="12.7545454545455" customWidth="1"/>
   </cols>
@@ -3467,7 +4111,7 @@
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C1">
         <v>0.4</v>
@@ -3487,16 +4131,16 @@
       <c r="H1">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>120</v>
+      <c r="I1" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -3516,8 +4160,37 @@
       <c r="H2">
         <v>15</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>46590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>46842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>